<commit_message>
Plot de resultados e Randomized Search
</commit_message>
<xml_diff>
--- a/TCC2/Results/Teste_0_importance.xlsx
+++ b/TCC2/Results/Teste_0_importance.xlsx
@@ -533,28 +533,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.05327415797539324</v>
+        <v>0.05036926603476129</v>
       </c>
       <c r="C3" t="n">
-        <v>0.04523145030390987</v>
+        <v>0.04810577851090812</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2612823607478387</v>
+        <v>0.2593900765466494</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1634574075136959</v>
+        <v>0.1638837631406302</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2836876442198095</v>
+        <v>0.2822226973097523</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0289103716842631</v>
+        <v>0.03063995123661579</v>
       </c>
       <c r="H3" t="n">
-        <v>0.008734639573603554</v>
+        <v>0.009700816207382813</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1554219679814863</v>
+        <v>0.1556876510133002</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -615,28 +615,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6329166974694475</v>
+        <v>0.6327793089254982</v>
       </c>
       <c r="C5" t="n">
-        <v>0.006463320396543767</v>
+        <v>0.006783646948945634</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1069563332315876</v>
+        <v>0.1066881310663325</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01472130627497678</v>
+        <v>0.01540081225901808</v>
       </c>
       <c r="F5" t="n">
-        <v>0.166694361733796</v>
+        <v>0.1660904133886679</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00831072281251966</v>
+        <v>0.008363622570634641</v>
       </c>
       <c r="H5" t="n">
-        <v>0.003236745950399998</v>
+        <v>0.003428890017103599</v>
       </c>
       <c r="I5" t="n">
-        <v>0.06070051213072888</v>
+        <v>0.06046517482379939</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -697,28 +697,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.03616509674372524</v>
+        <v>0.02960493329126054</v>
       </c>
       <c r="C7" t="n">
-        <v>0.02838676533310112</v>
+        <v>0.03483615317030731</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3092547667343902</v>
+        <v>0.3106804032362739</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1125662635104972</v>
+        <v>0.1120979159246963</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2616088190620295</v>
+        <v>0.260766600949732</v>
       </c>
       <c r="G7" t="n">
-        <v>0.03205671819827949</v>
+        <v>0.03198024842939234</v>
       </c>
       <c r="H7" t="n">
-        <v>0.008048957964381719</v>
+        <v>0.00806672596056306</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2119126124535956</v>
+        <v>0.2119670190377746</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -779,28 +779,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.03955214101192617</v>
+        <v>0.037671776761382</v>
       </c>
       <c r="C9" t="n">
-        <v>0.03600444568293461</v>
+        <v>0.03819856916820293</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3900065614147335</v>
+        <v>0.3900002457404643</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1021163464826955</v>
+        <v>0.1031396469016726</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2166593771766614</v>
+        <v>0.2153208856039616</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0422302553466975</v>
+        <v>0.04245174602176691</v>
       </c>
       <c r="H9" t="n">
-        <v>0.005919543440464735</v>
+        <v>0.005802853835911848</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1675113294438866</v>
+        <v>0.167414275966638</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -861,28 +861,28 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1643106026873019</v>
+        <v>0.1449532778103223</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1580935532237618</v>
+        <v>0.1758429575723237</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1606228640377437</v>
+        <v>0.1583528749052667</v>
       </c>
       <c r="E11" t="n">
-        <v>0.03250238493540041</v>
+        <v>0.03332820444540429</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2262468134232483</v>
+        <v>0.2437663247539522</v>
       </c>
       <c r="G11" t="n">
-        <v>0.02121698426927618</v>
+        <v>0.02175476080943349</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1481215069991147</v>
+        <v>0.1347931964070899</v>
       </c>
       <c r="I11" t="n">
-        <v>0.08888529042415293</v>
+        <v>0.08720840329620741</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -949,22 +949,22 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.217754316178691</v>
+        <v>0.2194636015344086</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1558510296631271</v>
+        <v>0.1583395034170087</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3390216202846408</v>
+        <v>0.3342732968973308</v>
       </c>
       <c r="G13" t="n">
-        <v>0.02742867628046103</v>
+        <v>0.02803793712424213</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0004000990153790009</v>
+        <v>0.0003563260142842282</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2595442585777012</v>
+        <v>0.2595293350127256</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>

</xml_diff>